<commit_message>
Changes Pre Driver Fun Imp
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.3\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8D68DF-411B-48DC-9212-F2EB5933D427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9827FEA-C8B8-4A38-A17D-40B14F195650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="720" windowWidth="15750" windowHeight="14310" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Motions" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
   <si>
     <t>Mass</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>spj (global)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Driver (Equations must be defined has handles @(variable) function)</t>
   </si>
 </sst>
 </file>
@@ -379,7 +385,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -477,31 +483,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,24 +559,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,7 +574,25 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -627,16 +613,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1044,18 +1024,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1065,10 +1045,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1078,10 +1058,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1091,10 +1071,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1110,18 +1090,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1130,10 +1110,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1148,58 +1128,58 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1207,11 +1187,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B11:C11"/>
@@ -1221,6 +1196,11 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4765,7 +4745,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="I45" sqref="I45:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4824,11 +4804,11 @@
       <c r="E2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4966,21 +4946,21 @@
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50" t="s">
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5099,16 +5079,16 @@
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="50" t="s">
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5223,16 +5203,16 @@
       <c r="E16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50" t="s">
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
@@ -5306,16 +5286,16 @@
       <c r="E20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50" t="s">
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
     </row>
     <row r="21" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
@@ -5354,19 +5334,19 @@
     </row>
     <row r="22" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
     </row>
     <row r="24" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
@@ -5384,16 +5364,16 @@
       <c r="E24" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="54"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="53" t="s">
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="J24" s="54"/>
-      <c r="K24" s="55"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
     </row>
     <row r="25" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I25" s="10"/>
@@ -5525,7 +5505,7 @@
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>1</v>
       </c>
@@ -5546,7 +5526,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -5559,7 +5539,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -5573,9 +5553,9 @@
       <c r="K35" s="4"/>
       <c r="L35" s="9"/>
     </row>
-    <row r="36" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
@@ -5588,7 +5568,7 @@
       <c r="J36" s="48"/>
       <c r="K36" s="48"/>
     </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>62</v>
       </c>
@@ -5613,13 +5593,13 @@
       <c r="H37" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="50" t="s">
+      <c r="I37" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-    </row>
-    <row r="38" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+    </row>
+    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>2</v>
       </c>
@@ -5654,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -5667,7 +5647,7 @@
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="48" t="s">
         <v>28</v>
       </c>
@@ -5678,7 +5658,7 @@
       <c r="F40" s="48"/>
       <c r="G40" s="48"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>62</v>
       </c>
@@ -5691,13 +5671,13 @@
       <c r="D41" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="50" t="s">
+      <c r="E41" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <v>1</v>
       </c>
@@ -5719,8 +5699,11 @@
       <c r="G42" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <v>2</v>
       </c>
@@ -5743,7 +5726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
         <v>3</v>
       </c>
@@ -5766,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <v>4</v>
       </c>
@@ -5789,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -5801,6 +5784,18 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="A40:G40"/>
     <mergeCell ref="E41:G41"/>
     <mergeCell ref="A19:K19"/>
@@ -5813,18 +5808,6 @@
     <mergeCell ref="A23:K23"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35 B18 B38:B39" xr:uid="{00000000-0002-0000-0100-000001000000}">

</xml_diff>

<commit_message>
Changes pre  Input Imp 16 03
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.3\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9827FEA-C8B8-4A38-A17D-40B14F195650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F802253-6F3E-49DB-8FBF-BC6093CBEEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
   <si>
     <t>Mass</t>
   </si>
@@ -227,12 +227,6 @@
     <t>Rotational input</t>
   </si>
   <si>
-    <t>v0/w0</t>
-  </si>
-  <si>
-    <t>a0/gamma</t>
-  </si>
-  <si>
     <t>Input T3 - Orientational Axis of Rot</t>
   </si>
   <si>
@@ -284,7 +278,13 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Driver (Equations must be defined has handles @(variable) function)</t>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Driver (Equations must be defined has handles @(variable) function) [Rot Inputs in Radians]</t>
+  </si>
+  <si>
+    <t>@(t) 0,523 + 0,3*t</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -559,6 +559,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,25 +592,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,10 +613,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -626,6 +626,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1024,18 +1045,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1045,10 +1066,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1058,10 +1079,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="41"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1071,10 +1092,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1090,18 +1111,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1110,10 +1131,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1128,58 +1149,58 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="41"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="41"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1187,6 +1208,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B11:C11"/>
@@ -1196,11 +1222,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1212,7 +1233,7 @@
   <dimension ref="A1:AB197"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1272,7 @@
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
       <c r="O1" s="44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P1" s="44"/>
       <c r="Q1" s="44"/>
@@ -1508,7 +1529,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="22">
         <v>467.13</v>
@@ -1576,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="21">
         <v>700</v>
@@ -4744,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45:I46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4753,6 +4774,7 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
@@ -4804,11 +4826,11 @@
       <c r="E2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="F2" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4831,7 +4853,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -4946,21 +4968,21 @@
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -4977,7 +4999,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="18">
         <v>3</v>
@@ -5079,16 +5101,16 @@
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
+      <c r="F11" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5105,7 +5127,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D12" s="18">
         <v>1</v>
@@ -5203,16 +5225,16 @@
       <c r="E16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
+      <c r="F16" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
@@ -5286,16 +5308,16 @@
       <c r="E20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="49" t="s">
+      <c r="F20" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
     </row>
     <row r="21" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
@@ -5305,7 +5327,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D21" s="24">
         <v>4</v>
@@ -5335,7 +5357,7 @@
     <row r="22" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
@@ -5365,12 +5387,12 @@
         <v>16</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="52"/>
       <c r="H24" s="53"/>
       <c r="I24" s="51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J24" s="52"/>
       <c r="K24" s="53"/>
@@ -5554,19 +5576,19 @@
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
+      <c r="A36" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
     <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -5582,22 +5604,16 @@
         <v>23</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G37" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="H37" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I37" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="56"/>
     </row>
     <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
@@ -5612,25 +5628,19 @@
       <c r="D38" s="18">
         <v>2</v>
       </c>
-      <c r="E38" s="18">
-        <v>0.52300000000000002</v>
+      <c r="E38" s="60" t="s">
+        <v>83</v>
       </c>
       <c r="F38" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="G38" s="18">
-        <v>0</v>
-      </c>
-      <c r="H38" s="18">
         <v>6</v>
       </c>
+      <c r="G38" s="12">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
       <c r="I38" s="12">
-        <v>0</v>
-      </c>
-      <c r="J38" s="12">
-        <v>0</v>
-      </c>
-      <c r="K38" s="12">
         <v>1</v>
       </c>
     </row>
@@ -5671,18 +5681,18 @@
       <c r="D41" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <v>1</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>26</v>
@@ -5700,7 +5710,7 @@
         <v>0</v>
       </c>
       <c r="M42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -5708,10 +5718,10 @@
         <v>2</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D43" s="18">
         <v>2</v>
@@ -5731,10 +5741,10 @@
         <v>3</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D44" s="18">
         <v>3</v>
@@ -5754,10 +5764,10 @@
         <v>4</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D45" s="18">
         <v>4</v>
@@ -5784,18 +5794,6 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="A40:G40"/>
     <mergeCell ref="E41:G41"/>
     <mergeCell ref="A19:K19"/>
@@ -5803,11 +5801,23 @@
     <mergeCell ref="I20:K20"/>
     <mergeCell ref="A27:F27"/>
     <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="I37:K37"/>
     <mergeCell ref="A23:K23"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35 B18 B38:B39" xr:uid="{00000000-0002-0000-0100-000001000000}">

</xml_diff>

<commit_message>
Version that now reads Functions as Inputs
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.3\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F802253-6F3E-49DB-8FBF-BC6093CBEEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CFDABE-E553-4F7E-A6C9-AB734A6A5045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18825" yWindow="7830" windowWidth="15750" windowHeight="14310" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Motions" sheetId="4" r:id="rId1"/>
     <sheet name="Bodies" sheetId="1" r:id="rId2"/>
     <sheet name="Joints" sheetId="2" r:id="rId3"/>
+    <sheet name="Joints_Drivers" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="85">
   <si>
     <t>Mass</t>
   </si>
@@ -230,9 +231,6 @@
     <t>Input T3 - Orientational Axis of Rot</t>
   </si>
   <si>
-    <t>Rotational Axis (vector)</t>
-  </si>
-  <si>
     <t>Point</t>
   </si>
   <si>
@@ -284,7 +282,13 @@
     <t>Driver (Equations must be defined has handles @(variable) function) [Rot Inputs in Radians]</t>
   </si>
   <si>
-    <t>@(t) 0,523 + 0,3*t</t>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Vector Direction/Rotational Axis</t>
+  </si>
+  <si>
+    <t>@(t) 0.523 - 0.3*t</t>
   </si>
 </sst>
 </file>
@@ -487,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -554,6 +558,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1034,7 +1041,7 @@
   <dimension ref="B3:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="G26" sqref="G25:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,18 +1052,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1066,10 +1073,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1079,10 +1086,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1092,10 +1099,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1111,18 +1118,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1131,10 +1138,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1149,58 +1156,58 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1251,78 +1258,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="43"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44" t="s">
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44" t="s">
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44" t="s">
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="46" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44" t="s">
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44" t="s">
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="47" t="s">
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="46" t="s">
+      <c r="S2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1376,8 +1383,8 @@
       <c r="Q3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="47"/>
-      <c r="S3" s="45"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="46"/>
       <c r="T3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1529,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="22">
         <v>467.13</v>
@@ -1597,7 +1604,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="21">
         <v>700</v>
@@ -4765,8 +4772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4786,16 +4793,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4826,11 +4833,11 @@
       <c r="E2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="F2" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4853,7 +4860,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -4928,22 +4935,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -4968,21 +4975,21 @@
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50" t="s">
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -4999,7 +5006,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="18">
         <v>3</v>
@@ -5064,19 +5071,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5101,16 +5108,16 @@
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
+      <c r="F11" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5127,7 +5134,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="18">
         <v>1</v>
@@ -5188,19 +5195,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5225,16 +5232,16 @@
       <c r="E16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
@@ -5271,19 +5278,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5308,16 +5315,16 @@
       <c r="E20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50" t="s">
+      <c r="F20" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
     </row>
     <row r="21" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
@@ -5327,7 +5334,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="24">
         <v>4</v>
@@ -5356,19 +5363,19 @@
     </row>
     <row r="22" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
+      <c r="A23" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
     </row>
     <row r="24" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
@@ -5386,16 +5393,16 @@
       <c r="E24" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="F24" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="52"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="J24" s="52"/>
-      <c r="K24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="54"/>
     </row>
     <row r="25" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I25" s="10"/>
@@ -5404,14 +5411,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5485,12 +5492,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5561,225 +5568,148 @@
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+    <row r="35" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="10"/>
       <c r="K35" s="4"/>
       <c r="L35" s="9"/>
     </row>
-    <row r="36" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="59"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
     </row>
     <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="54" t="s">
+      <c r="A37" s="18">
+        <v>1</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56"/>
+      <c r="C37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="18">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18">
+        <v>0</v>
+      </c>
+      <c r="F37" s="18">
+        <v>0</v>
+      </c>
+      <c r="G37" s="18">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>2</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D38" s="18">
         <v>2</v>
       </c>
-      <c r="E38" s="60" t="s">
-        <v>83</v>
+      <c r="E38" s="18">
+        <v>173.2</v>
       </c>
       <c r="F38" s="18">
-        <v>6</v>
-      </c>
-      <c r="G38" s="12">
-        <v>0</v>
-      </c>
-      <c r="H38" s="12">
-        <v>0</v>
-      </c>
-      <c r="I38" s="12">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G38" s="18">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
+      <c r="A39" s="18">
+        <v>3</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="18">
+        <v>3</v>
+      </c>
+      <c r="E39" s="18">
+        <v>663</v>
+      </c>
+      <c r="F39" s="18">
+        <v>0</v>
+      </c>
+      <c r="G39" s="18">
+        <v>0</v>
+      </c>
       <c r="H39"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="18">
+        <v>4</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="18">
+        <v>4</v>
+      </c>
+      <c r="E40" s="18">
+        <v>763</v>
+      </c>
+      <c r="F40" s="18">
+        <v>0</v>
+      </c>
+      <c r="G40" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
-        <v>1</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="18">
-        <v>1</v>
-      </c>
-      <c r="E42" s="18">
-        <v>0</v>
-      </c>
-      <c r="F42" s="18">
-        <v>0</v>
-      </c>
-      <c r="G42" s="18">
-        <v>0</v>
-      </c>
       <c r="M42" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="18">
-        <v>2</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="18">
-        <v>2</v>
-      </c>
-      <c r="E43" s="18">
-        <v>173.2</v>
-      </c>
-      <c r="F43" s="18">
-        <v>100</v>
-      </c>
-      <c r="G43" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="18">
-        <v>3</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="18">
-        <v>3</v>
-      </c>
-      <c r="E44" s="18">
-        <v>663</v>
-      </c>
-      <c r="F44" s="18">
-        <v>0</v>
-      </c>
-      <c r="G44" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="18">
-        <v>4</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="18">
-        <v>4</v>
-      </c>
-      <c r="E45" s="18">
-        <v>763</v>
-      </c>
-      <c r="F45" s="18">
-        <v>0</v>
-      </c>
-      <c r="G45" s="18">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -5793,9 +5723,8 @@
     </row>
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="E41:G41"/>
+  <mergeCells count="22">
+    <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:K20"/>
@@ -5804,8 +5733,7 @@
     <mergeCell ref="A23:K23"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A35:G35"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="I11:K11"/>
@@ -5820,11 +5748,11 @@
     <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35 B18 B38:B39" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Spherical,Universal,Revolute,Translation,Cylindrical,Simple,Ground,Driver"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B1032" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46:B1032 B37:B40" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Spherical,Universal,Revolute,Cylindrical,Translation,Simple,Driver,Ground,Point"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5832,4 +5760,106 @@
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4658AC4-6667-4045-B0FE-42E281567C35}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="56"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="18">
+        <v>2</v>
+      </c>
+      <c r="E3" s="18">
+        <v>6</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{2127DDA1-6D8E-4B00-8D96-D683E7741146}">
+      <formula1>"Spherical,Universal,Revolute,Translation,Cylindrical,Simple,Ground,Driver"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sinusoidal and Poly Implemented
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.3\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CFDABE-E553-4F7E-A6C9-AB734A6A5045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E244A0-9641-4059-BAE7-5682B8604C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18825" yWindow="7830" windowWidth="15750" windowHeight="14310" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Motions" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
   <si>
     <t>Mass</t>
   </si>
@@ -288,7 +288,13 @@
     <t>Vector Direction/Rotational Axis</t>
   </si>
   <si>
-    <t>@(t) 0.523 - 0.3*t</t>
+    <t>@(t)sin(5*t)</t>
+  </si>
+  <si>
+    <t>Function Type (Sinusoidal or Polynomial)</t>
+  </si>
+  <si>
+    <t>Sinusoidal</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -487,11 +493,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,22 +581,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -599,7 +599,25 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -617,13 +635,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -635,6 +653,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,16 +671,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1052,18 +1076,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1073,10 +1097,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="42"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1086,10 +1110,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1099,10 +1123,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1118,18 +1142,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="37"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1138,10 +1162,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1156,58 +1180,58 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1215,11 +1239,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B11:C11"/>
@@ -1229,6 +1248,11 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1258,78 +1282,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45" t="s">
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45" t="s">
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45" t="s">
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="47" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47" t="s">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47" t="s">
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="45" t="s">
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45" t="s">
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="48" t="s">
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="47" t="s">
+      <c r="S2" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1383,8 +1407,8 @@
       <c r="Q3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="48"/>
-      <c r="S3" s="46"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="47"/>
       <c r="T3" s="21" t="s">
         <v>4</v>
       </c>
@@ -4793,16 +4817,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4833,11 +4857,11 @@
       <c r="E2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4935,22 +4959,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -4975,21 +4999,21 @@
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51" t="s">
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51" t="s">
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5071,19 +5095,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5108,16 +5132,16 @@
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51" t="s">
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5195,19 +5219,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5232,16 +5256,16 @@
       <c r="E16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51" t="s">
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
@@ -5278,19 +5302,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5315,16 +5339,16 @@
       <c r="E20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
     </row>
     <row r="21" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
@@ -5363,19 +5387,19 @@
     </row>
     <row r="22" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
     </row>
     <row r="24" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
@@ -5393,16 +5417,16 @@
       <c r="E24" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F24" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="G24" s="53"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="52" t="s">
+      <c r="G24" s="54"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="J24" s="53"/>
-      <c r="K24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="55"/>
     </row>
     <row r="25" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I25" s="10"/>
@@ -5411,14 +5435,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5492,12 +5516,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5569,15 +5593,15 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="60"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="58"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="10"/>
@@ -5597,11 +5621,11 @@
       <c r="D36" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -5724,6 +5748,18 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -5734,18 +5770,6 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -5764,10 +5788,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4658AC4-6667-4045-B0FE-42E281567C35}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5777,22 +5801,24 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="10" max="10" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>62</v>
       </c>
@@ -5808,16 +5834,19 @@
       <c r="E2" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="57"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="31" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -5842,17 +5871,20 @@
       <c r="H3" s="12">
         <v>1</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="I3" s="32" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I4" s="61"/>
+      <c r="J3" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
     <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{2127DDA1-6D8E-4B00-8D96-D683E7741146}">

</xml_diff>

<commit_message>
Changes 19 03, pK Opt
</commit_message>
<xml_diff>
--- a/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
+++ b/pK-EP-v.1.0.3/Excel Files/crank_slide_2D_Nikra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\pK-EP-v.1.0.3\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CB7721-BCD3-4E72-8543-D9C81FC0B5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F764941E-13B3-4ADC-B9DF-0882244FEF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7860" yWindow="1110" windowWidth="15750" windowHeight="14310" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -291,10 +291,10 @@
     <t>Function Type (Sinusoidal or Polynomial)</t>
   </si>
   <si>
-    <t>@(t)0.523+0.3*t</t>
-  </si>
-  <si>
     <t>Polynomial</t>
+  </si>
+  <si>
+    <t>@(t)0.523-0.3*t</t>
   </si>
 </sst>
 </file>
@@ -587,6 +587,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,25 +620,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -638,13 +638,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1076,18 +1076,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="13">
         <v>0</v>
       </c>
@@ -1097,10 +1097,10 @@
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="13">
         <v>0</v>
       </c>
@@ -1110,10 +1110,10 @@
       <c r="S5" s="16"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="13">
         <v>0</v>
       </c>
@@ -1123,10 +1123,10 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="13">
         <v>0</v>
       </c>
@@ -1142,18 +1142,18 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="17">
         <v>2</v>
       </c>
@@ -1162,10 +1162,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="17">
         <v>0.5</v>
       </c>
@@ -1180,58 +1180,58 @@
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="44"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
         <v>41</v>
@@ -1239,6 +1239,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B11:C11"/>
@@ -1248,11 +1253,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4817,16 +4817,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -4857,11 +4857,11 @@
       <c r="E2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4959,22 +4959,22 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
@@ -4999,21 +4999,21 @@
       <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="51" t="s">
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51" t="s">
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -5095,19 +5095,19 @@
       <c r="X9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5132,16 +5132,16 @@
       <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="51" t="s">
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -5219,19 +5219,19 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5256,16 +5256,16 @@
       <c r="E16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="51" t="s">
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
     </row>
     <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
@@ -5302,19 +5302,19 @@
       <c r="X18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -5339,16 +5339,16 @@
       <c r="E20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="51" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
     </row>
     <row r="21" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
@@ -5387,19 +5387,19 @@
     </row>
     <row r="22" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
     </row>
     <row r="24" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
@@ -5435,14 +5435,14 @@
     </row>
     <row r="26" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -5516,12 +5516,12 @@
       <c r="X30" s="10"/>
     </row>
     <row r="31" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -5621,11 +5621,11 @@
       <c r="D36" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="10"/>
@@ -5748,18 +5748,6 @@
     <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="A19:K19"/>
     <mergeCell ref="F20:H20"/>
@@ -5770,6 +5758,18 @@
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -5791,7 +5791,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5872,10 +5872,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>